<commit_message>
transformed into webapage with Flask
</commit_message>
<xml_diff>
--- a/lead_report.xlsx
+++ b/lead_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/pages/contact-us</t>
+          <t>https://www.luggagepros.com//pages/contact-us</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -488,146 +488,138 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://shop.samsonite.com/</t>
+          <t>https://luggagehero.com/san-francisco/12th-st-oakland/</t>
         </is>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>questions@samsonite.com</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://shop.samsonite.com/contact-us.html</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>https://luggagehero.com/san-francisco/12th-st-oakland/https://luggagehero.com/contact-us/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>intercom</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://luggagehero.com/oakland/</t>
+          <t>https://shop.samsonite.com/</t>
         </is>
       </c>
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>questions@samsonite.com</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://luggagehero.com/contact-us/</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>intercom</t>
-        </is>
-      </c>
+          <t>https://shop.samsonite.com/https://shop.samsonite.com/contact-us.html</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://luggagehero.com/san-francisco/12th-st-oakland/</t>
+          <t>https://www.goodhousekeeping.com/travel-products/g26898407/best-luggage-brands/#:~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years.</t>
         </is>
       </c>
       <c r="B5" t="b">
         <v>0</v>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>lsachs@hearst.com</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://luggagehero.com/contact-us/</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>intercom</t>
-        </is>
-      </c>
+          <t>https://www.goodhousekeeping.com/travel-products/g26898407/best-luggage-brands/#:~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years./about/a18834/contact-us/</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.tumi.com/</t>
+          <t>https://www.storespace.com/tips-advice/storage/packing-hacks/8-luggage-suitcase-storage-tips#:~:text=In%20the%20closet,the%20side%20against%20the%20wall.</t>
         </is>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://www.storespace.com/tips-advice/storage/packing-hacks/8-luggage-suitcase-storage-tips#:~:text=In%20the%20closet,the%20side%20against%20the%20wall.#</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://lazarsluggage.com/</t>
+          <t>https://www.samsonite.co.za/faq/#:~:text=WHERE%20CAN%20I%20FIND%20MY,the%20inside%20of%20your%20product.</t>
         </is>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>info@lazarsluggage.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>/pages/contact</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.briggs-riley.com/</t>
+          <t>https://uk.tumi.com/tumi-difference.html#:~:text=What%20Makes%20Us%20Different,solutions%20for%20today%20and%20beyond.</t>
         </is>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>/pages/customer-service</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>zendesk</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>name@domain.com</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.luggagefactory.com/</t>
+          <t>https://luggagehero.com/oakland/</t>
         </is>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Untitled-2_cda00be6-b25a-4f4e-87a8-17254b5ee507_500x@2x.jpg</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.luggagefactory.com/pages/contact-us</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>https://luggagehero.com/oakland/https://luggagehero.com/contact-us/</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>intercom</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.nordstrom.com/browse/home/luggage-travel</t>
+          <t>https://www.tumi.com/</t>
         </is>
       </c>
       <c r="B10" t="b">
@@ -640,129 +632,23 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://usebounce.com/city/oakland</t>
+          <t>https://www.luggagefactory.com/</t>
         </is>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>team@usebounce.com</t>
+          <t>Untitled-2_cda00be6-b25a-4f4e-87a8-17254b5ee507_500x@2x.jpg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>/support</t>
+          <t>https://www.luggagefactory.com/https://www.luggagefactory.com/pages/contact-us</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>https://www.swissgear.com/</t>
-        </is>
-      </c>
-      <c r="B12" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>email@address.com</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>https://www.swissgear.com/contact</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://www.target.com/c/luggage/-/N-5xtz1</t>
-        </is>
-      </c>
-      <c r="B13" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>https://store.ricksteves.com/shop/travel-bags</t>
-        </is>
-      </c>
-      <c r="B14" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>https://www.ricksteves.com/about-us/contact-us</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>https://www.macys.com/shop/luggage?id=16908</t>
-        </is>
-      </c>
-      <c r="B15" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>https://www.awaytravel.com/</t>
-        </is>
-      </c>
-      <c r="B16" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>help@awaytravel.com</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>https://help.awaytravel.co.uk/contact/form-BJG0_IjZn</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>https://luggagecenter.com/</t>
-        </is>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>LC-Logo_140x@2x.jpg</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>/pages/contact-us</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore: Update timeout for requests to 3 seconds
```
</commit_message>
<xml_diff>
--- a/lead_report.xlsx
+++ b/lead_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>URL</t>
   </si>
@@ -31,70 +31,181 @@
     <t>Live_Chat_Solution</t>
   </si>
   <si>
-    <t>https://shop.samsonite.com/</t>
-  </si>
-  <si>
-    <t>https://www.luggagepros.com/</t>
-  </si>
-  <si>
-    <t>https://www.unclaimedbaggage.com/</t>
-  </si>
-  <si>
-    <t>https://luggagehero.com/oakland/</t>
-  </si>
-  <si>
-    <t>https://luggagehero.com/san-francisco/12th-st-oakland/</t>
-  </si>
-  <si>
-    <t>https://www.nordstrom.com/browse/home/luggage-travel</t>
-  </si>
-  <si>
-    <t>https://www.goodhousekeeping.com/travel-products/g26898407/best-luggage-brands/#:~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years.</t>
-  </si>
-  <si>
-    <t>https://www.storespace.com/tips-advice/storage/packing-hacks/8-luggage-suitcase-storage-tips#:~:text=In%20the%20closet,the%20side%20against%20the%20wall.</t>
-  </si>
-  <si>
-    <t>https://www.samsonite.co.za/faq/#:~:text=WHERE%20CAN%20I%20FIND%20MY,the%20inside%20of%20your%20product.</t>
-  </si>
-  <si>
-    <t>https://www.tumi.com/</t>
-  </si>
-  <si>
-    <t>questions@samsonite.com</t>
-  </si>
-  <si>
-    <t>luggage@luggagepros.com</t>
-  </si>
-  <si>
-    <t>lsachs@hearst.com</t>
-  </si>
-  <si>
-    <t>https://shop.samsonite.com/contact-us.html</t>
-  </si>
-  <si>
-    <t>https://www.luggagepros.com//pages/contact-us</t>
-  </si>
-  <si>
-    <t>https://www.unclaimedbaggage.com//pages/contact</t>
-  </si>
-  <si>
-    <t>https://luggagehero.com/contact-us/</t>
-  </si>
-  <si>
-    <t>https://www.goodhousekeeping.com/travel-products/g26898407/best-luggage-brands/#:~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years./about/a18834/contact-us/</t>
-  </si>
-  <si>
-    <t>https://www.storespace.com/tips-advice/storage/packing-hacks/8-luggage-suitcase-storage-tips#:~:text=In%20the%20closet,the%20side%20against%20the%20wall.#</t>
-  </si>
-  <si>
-    <t>tidio</t>
-  </si>
-  <si>
-    <t>richpanel</t>
-  </si>
-  <si>
-    <t>intercom</t>
+    <t>https://www.lawinsider.com/dictionary/fashion-accessory-stores#:~:text=Fashion%20Accessory%20Stores%20means%20stores,accessories%20and%20other%20fashion%20accessories.</t>
+  </si>
+  <si>
+    <t>https://growfers.com/story/claires/#:~:text=Because%20wigs%20were%20no%20longer,which%20every%20girl%20will%20like.</t>
+  </si>
+  <si>
+    <t>https://www.comparably.com/companies/charming-charlie/competitors#:~:text=charming%20charlie%20competitors%20include%20Kendra,Forever%2021%20and%20Charlotte%20Russe.</t>
+  </si>
+  <si>
+    <t>https://www.claires.com/</t>
+  </si>
+  <si>
+    <t>https://charmingcharlie.com/</t>
+  </si>
+  <si>
+    <t>https://www.accessorizeeveryone.net/</t>
+  </si>
+  <si>
+    <t>https://beachwaver.com/collections/theaccessoryshop</t>
+  </si>
+  <si>
+    <t>https://www.youraccessoryshop.com/</t>
+  </si>
+  <si>
+    <t>https://thetreasuredaccessory.com/</t>
+  </si>
+  <si>
+    <t>https://accessories.ford.com/</t>
+  </si>
+  <si>
+    <t>https://www.anthropologie.com/shoes-accessories</t>
+  </si>
+  <si>
+    <t>https://www.reddit.com/r/VALORANT/comments/18ztfo7/accesory_shop/</t>
+  </si>
+  <si>
+    <t>https://www.spartan.com/collections/accessories-shop-all</t>
+  </si>
+  <si>
+    <t>https://www.cornellstore.com/accessories/</t>
+  </si>
+  <si>
+    <t>https://www.schiaparelli.com/eshop/en/e-shop/accessories/c/000038</t>
+  </si>
+  <si>
+    <t>https://shop.siriusxm.com/all-accessories/</t>
+  </si>
+  <si>
+    <t>https://www.shopdoen.com/collections/accessories</t>
+  </si>
+  <si>
+    <t>https://shop.invisalign.com/collections/accessories</t>
+  </si>
+  <si>
+    <t>https://www.netflix.shop/collections/accessories</t>
+  </si>
+  <si>
+    <t>https://accessory.qnap.com/</t>
+  </si>
+  <si>
+    <t>https://www.vitra.com/en-us/product/category/accessories</t>
+  </si>
+  <si>
+    <t>https://shop.in-n-out.com/collections/specialty-items</t>
+  </si>
+  <si>
+    <t>https://vwaccessoriesshop.com/</t>
+  </si>
+  <si>
+    <t>https://shop.berninausa.com/all-accessories</t>
+  </si>
+  <si>
+    <t>https://paparazziaccessories.com/</t>
+  </si>
+  <si>
+    <t>https://shop.bmwusa.com/vehicle-accessories.html</t>
+  </si>
+  <si>
+    <t>https://www.apple.com/shop/accessories/all</t>
+  </si>
+  <si>
+    <t>https://shop.equinox.com/collections/accessories</t>
+  </si>
+  <si>
+    <t>your@email.com</t>
+  </si>
+  <si>
+    <t>9f057df6115a4bb488c08ea12a835e6e@o418887.ingest.sentry.io</t>
+  </si>
+  <si>
+    <t>flags@2x.png</t>
+  </si>
+  <si>
+    <t>username@domain.com</t>
+  </si>
+  <si>
+    <t>form_radio@2x.png</t>
+  </si>
+  <si>
+    <t>privacy@vitra.com</t>
+  </si>
+  <si>
+    <t>contact@vwaccessoriesshop.com</t>
+  </si>
+  <si>
+    <t>bernina@indition.com</t>
+  </si>
+  <si>
+    <t>example@email.com</t>
+  </si>
+  <si>
+    <t>231206_EquinoxShop4646-lpr_3b6e54ed-046d-4e39-90c1-125bfe7b8b46_370x230@2x.jpg</t>
+  </si>
+  <si>
+    <t>https://www.lawinsider.com/dictionary/fashion-accessory-stores#:~:text=Fashion%20Accessory%20Stores%20means%20stores,accessories%20and%20other%20fashion%20accessories./dictionary/airport-ground-support-equipment</t>
+  </si>
+  <si>
+    <t>https://www.claires.com/customer-service-contact/?lang=en_GB</t>
+  </si>
+  <si>
+    <t>https://charmingcharlie.com//pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://beachwaver.com/pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://thetreasuredaccessory.com//pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://spartanrace.zendesk.com/hc/en-us/requests/new</t>
+  </si>
+  <si>
+    <t>https://www.cornellstore.com/accessories//faculty-support</t>
+  </si>
+  <si>
+    <t>https://www.schiaparelli.com/eshop/en/contact-us</t>
+  </si>
+  <si>
+    <t>https://shop.siriusxm.com/all-accessories//contact-us.html</t>
+  </si>
+  <si>
+    <t>https://www.shopdoen.com/collections/accessories/pages/contact</t>
+  </si>
+  <si>
+    <t>https://shop.invisalign.com/pages/contact-us</t>
+  </si>
+  <si>
+    <t>https://help.netflixshopsupport.com/hc/en-us</t>
+  </si>
+  <si>
+    <t>https://www.vitra.com/en-us/product/category/accessories/en-us/contact-service#Cat_Service</t>
+  </si>
+  <si>
+    <t>https://shop.in-n-out.com/collections/specialty-items/pages/contact</t>
+  </si>
+  <si>
+    <t>https://vwaccessoriesshop.com/contact-us/</t>
+  </si>
+  <si>
+    <t>https://www.bernina.com/en-US/Support-US</t>
+  </si>
+  <si>
+    <t>https://paparazziaccessories.com//contact/</t>
+  </si>
+  <si>
+    <t>https://shop.bmwusa.com/vehicle-accessories.html/content/shopbmwusa-com/us/en/support-and-policy/contact-now</t>
+  </si>
+  <si>
+    <t>https://www.apple.com/contact/</t>
+  </si>
+  <si>
+    <t>https://shop.equinox.com/collections/accessories/pages/contact-us</t>
+  </si>
+  <si>
+    <t>zendesk</t>
   </si>
 </sst>
 </file>
@@ -465,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,11 +606,8 @@
       <c r="B2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -507,16 +615,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -524,13 +623,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -541,10 +634,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -552,13 +642,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -574,13 +661,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -588,10 +675,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -599,7 +683,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -610,25 +700,275 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="D4" r:id="rId6"/>
-    <hyperlink ref="A5" r:id="rId7"/>
-    <hyperlink ref="D5" r:id="rId8"/>
-    <hyperlink ref="A6" r:id="rId9"/>
-    <hyperlink ref="D6" r:id="rId10"/>
-    <hyperlink ref="A7" r:id="rId11"/>
-    <hyperlink ref="A8" r:id="rId12" location=":~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years."/>
-    <hyperlink ref="D8" r:id="rId13" location=":~:text=Samsonite,-SHOP%20AT%20AMAZON&amp;text=Samsonite%20earns%20our%20top%20spot,tested%20it%20over%20the%20years./about/a18834/contact-us/"/>
-    <hyperlink ref="A9" r:id="rId14" location=":~:text=In%20the%20closet,the%20side%20against%20the%20wall."/>
-    <hyperlink ref="D9" r:id="rId15" location=":~:text=In%20the%20closet,the%20side%20against%20the%20wall.#"/>
-    <hyperlink ref="A10" r:id="rId16" location=":~:text=WHERE%20CAN%20I%20FIND%20MY,the%20inside%20of%20your%20product."/>
-    <hyperlink ref="A11" r:id="rId17"/>
+    <hyperlink ref="A2" r:id="rId1" location=":~:text=Fashion%20Accessory%20Stores%20means%20stores,accessories%20and%20other%20fashion%20accessories."/>
+    <hyperlink ref="D2" r:id="rId2" location=":~:text=Fashion%20Accessory%20Stores%20means%20stores,accessories%20and%20other%20fashion%20accessories./dictionary/airport-ground-support-equipment"/>
+    <hyperlink ref="A3" r:id="rId3" location=":~:text=Because%20wigs%20were%20no%20longer,which%20every%20girl%20will%20like."/>
+    <hyperlink ref="A4" r:id="rId4" location=":~:text=charming%20charlie%20competitors%20include%20Kendra,Forever%2021%20and%20Charlotte%20Russe."/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="D6" r:id="rId8"/>
+    <hyperlink ref="A7" r:id="rId9"/>
+    <hyperlink ref="A8" r:id="rId10"/>
+    <hyperlink ref="D8" r:id="rId11"/>
+    <hyperlink ref="A9" r:id="rId12"/>
+    <hyperlink ref="A10" r:id="rId13"/>
+    <hyperlink ref="D10" r:id="rId14"/>
+    <hyperlink ref="A11" r:id="rId15"/>
+    <hyperlink ref="A12" r:id="rId16"/>
+    <hyperlink ref="A13" r:id="rId17"/>
+    <hyperlink ref="A14" r:id="rId18"/>
+    <hyperlink ref="D14" r:id="rId19"/>
+    <hyperlink ref="A15" r:id="rId20"/>
+    <hyperlink ref="D15" r:id="rId21"/>
+    <hyperlink ref="A16" r:id="rId22"/>
+    <hyperlink ref="D16" r:id="rId23"/>
+    <hyperlink ref="A17" r:id="rId24"/>
+    <hyperlink ref="D17" r:id="rId25"/>
+    <hyperlink ref="A18" r:id="rId26"/>
+    <hyperlink ref="D18" r:id="rId27"/>
+    <hyperlink ref="A19" r:id="rId28"/>
+    <hyperlink ref="D19" r:id="rId29"/>
+    <hyperlink ref="A20" r:id="rId30"/>
+    <hyperlink ref="D20" r:id="rId31"/>
+    <hyperlink ref="A21" r:id="rId32"/>
+    <hyperlink ref="A22" r:id="rId33"/>
+    <hyperlink ref="D22" r:id="rId34" location="Cat_Service"/>
+    <hyperlink ref="A23" r:id="rId35"/>
+    <hyperlink ref="D23" r:id="rId36"/>
+    <hyperlink ref="A24" r:id="rId37"/>
+    <hyperlink ref="D24" r:id="rId38"/>
+    <hyperlink ref="A25" r:id="rId39"/>
+    <hyperlink ref="D25" r:id="rId40"/>
+    <hyperlink ref="A26" r:id="rId41"/>
+    <hyperlink ref="D26" r:id="rId42"/>
+    <hyperlink ref="A27" r:id="rId43"/>
+    <hyperlink ref="D27" r:id="rId44"/>
+    <hyperlink ref="A28" r:id="rId45"/>
+    <hyperlink ref="D28" r:id="rId46"/>
+    <hyperlink ref="A29" r:id="rId47"/>
+    <hyperlink ref="D29" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>